<commit_message>
Do all this on the construction job DONE -   Custom job def for a demolition job DONE - Add a demolition sprite DONE -  Hitting Go moves it to the bottom of the tile detail DONE -   Active jobs on this tile are shown when it is moved to DONE - In-Building Jobs DONE - Available jobs on this building are shown in the dropdown  DONE - Update the Dropdown to have Upgrade, DONE - New Demolition Job Object w/ no resources that sets the tile to "Nothing" or whatever I called it DONE - Update the Dropdown to have  Demo DONE - Update the Dropdown to have  New Job
</commit_message>
<xml_diff>
--- a/4xCityBuilder/Assets/Definitions/MergedSpreadsheet.xlsx
+++ b/4xCityBuilder/Assets/Definitions/MergedSpreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikeg\OneDrive\Documents\Documents\4XCityBuilder\4xCityBuilder\Assets\Definitions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD1F9F2-AFF0-4236-8207-4C4AAED36DAB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E59D93-83EA-4D39-A8C4-781AC51AD4D9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13560" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resources" sheetId="7" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3599" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3599" uniqueCount="571">
   <si>
     <t>Industry</t>
   </si>
@@ -1727,6 +1727,51 @@
   <si>
     <t>PMUs to Build</t>
   </si>
+  <si>
+    <t>Mine Copper Ore</t>
+  </si>
+  <si>
+    <t>Mine Tin Ore</t>
+  </si>
+  <si>
+    <t>Mine Silver Ore</t>
+  </si>
+  <si>
+    <t>Mine Gold Ore</t>
+  </si>
+  <si>
+    <t>Mine Iron Ore</t>
+  </si>
+  <si>
+    <t>Mine Adamantium Ore</t>
+  </si>
+  <si>
+    <t>Quarry Sandstone</t>
+  </si>
+  <si>
+    <t>Quarry Limestone</t>
+  </si>
+  <si>
+    <t>Quarry Marble</t>
+  </si>
+  <si>
+    <t>Quarry Granite</t>
+  </si>
+  <si>
+    <t>Gather Ash Wood</t>
+  </si>
+  <si>
+    <t>Gather Redwood</t>
+  </si>
+  <si>
+    <t>Gather Dryad-Wood</t>
+  </si>
+  <si>
+    <t>Gather Pine Wood</t>
+  </si>
+  <si>
+    <t>Gather Oak Wood</t>
+  </si>
 </sst>
 </file>
 
@@ -6720,7 +6765,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:W69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -19058,7 +19103,7 @@
       </c>
       <c r="B71" t="str">
         <f>JobBalancing!B72</f>
-        <v>Description</v>
+        <v>Gather Pine Wood</v>
       </c>
       <c r="C71">
         <f>JobBalancing!C72</f>
@@ -19208,7 +19253,7 @@
       </c>
       <c r="B72" t="str">
         <f>JobBalancing!B73</f>
-        <v>Description</v>
+        <v>Gather Oak Wood</v>
       </c>
       <c r="C72">
         <f>JobBalancing!C73</f>
@@ -20408,7 +20453,7 @@
       </c>
       <c r="B80" t="str">
         <f>JobBalancing!B81</f>
-        <v>Description</v>
+        <v>Mine Copper Ore</v>
       </c>
       <c r="C80">
         <f>JobBalancing!C81</f>
@@ -20558,7 +20603,7 @@
       </c>
       <c r="B81" t="str">
         <f>JobBalancing!B82</f>
-        <v>Description</v>
+        <v>Mine Tin Ore</v>
       </c>
       <c r="C81">
         <f>JobBalancing!C82</f>
@@ -20708,7 +20753,7 @@
       </c>
       <c r="B82" t="str">
         <f>JobBalancing!B83</f>
-        <v>Description</v>
+        <v>Mine Silver Ore</v>
       </c>
       <c r="C82">
         <f>JobBalancing!C83</f>
@@ -20858,7 +20903,7 @@
       </c>
       <c r="B83" t="str">
         <f>JobBalancing!B84</f>
-        <v>Description</v>
+        <v>Mine Gold Ore</v>
       </c>
       <c r="C83">
         <f>JobBalancing!C84</f>
@@ -21008,7 +21053,7 @@
       </c>
       <c r="B84" t="str">
         <f>JobBalancing!B85</f>
-        <v>Description</v>
+        <v>Mine Iron Ore</v>
       </c>
       <c r="C84">
         <f>JobBalancing!C85</f>
@@ -21158,7 +21203,7 @@
       </c>
       <c r="B85" t="str">
         <f>JobBalancing!B86</f>
-        <v>Description</v>
+        <v>Mine Adamantium Ore</v>
       </c>
       <c r="C85">
         <f>JobBalancing!C86</f>
@@ -21308,7 +21353,7 @@
       </c>
       <c r="B86" t="str">
         <f>JobBalancing!B87</f>
-        <v>Description</v>
+        <v>Quarry Sandstone</v>
       </c>
       <c r="C86">
         <f>JobBalancing!C87</f>
@@ -21458,7 +21503,7 @@
       </c>
       <c r="B87" t="str">
         <f>JobBalancing!B88</f>
-        <v>Description</v>
+        <v>Quarry Limestone</v>
       </c>
       <c r="C87">
         <f>JobBalancing!C88</f>
@@ -21608,7 +21653,7 @@
       </c>
       <c r="B88" t="str">
         <f>JobBalancing!B89</f>
-        <v>Description</v>
+        <v>Quarry Marble</v>
       </c>
       <c r="C88">
         <f>JobBalancing!C89</f>
@@ -21758,7 +21803,7 @@
       </c>
       <c r="B89" t="str">
         <f>JobBalancing!B90</f>
-        <v>Description</v>
+        <v>Quarry Granite</v>
       </c>
       <c r="C89">
         <f>JobBalancing!C90</f>
@@ -24758,7 +24803,7 @@
       </c>
       <c r="B109" t="str">
         <f>JobBalancing!B110</f>
-        <v>Description</v>
+        <v>Gather Ash Wood</v>
       </c>
       <c r="C109">
         <f>JobBalancing!C110</f>
@@ -24908,7 +24953,7 @@
       </c>
       <c r="B110" t="str">
         <f>JobBalancing!B111</f>
-        <v>Description</v>
+        <v>Gather Redwood</v>
       </c>
       <c r="C110">
         <f>JobBalancing!C111</f>
@@ -25058,7 +25103,7 @@
       </c>
       <c r="B111" t="str">
         <f>JobBalancing!B112</f>
-        <v>Description</v>
+        <v>Gather Dryad-Wood</v>
       </c>
       <c r="C111">
         <f>JobBalancing!C112</f>
@@ -31762,9 +31807,9 @@
   </sheetPr>
   <dimension ref="A1:BU117"/>
   <sheetViews>
-    <sheetView topLeftCell="Z1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BD10" sqref="BD10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -38253,7 +38298,7 @@
         <v>356</v>
       </c>
       <c r="B72" t="s">
-        <v>381</v>
+        <v>569</v>
       </c>
       <c r="C72">
         <v>1</v>
@@ -38294,7 +38339,7 @@
         <v>356</v>
       </c>
       <c r="B73" t="s">
-        <v>381</v>
+        <v>570</v>
       </c>
       <c r="C73">
         <v>2</v>
@@ -38733,7 +38778,7 @@
         <v>337</v>
       </c>
       <c r="B81" t="s">
-        <v>381</v>
+        <v>556</v>
       </c>
       <c r="C81">
         <v>2</v>
@@ -38774,7 +38819,7 @@
         <v>337</v>
       </c>
       <c r="B82" t="s">
-        <v>381</v>
+        <v>557</v>
       </c>
       <c r="C82">
         <v>2</v>
@@ -38815,7 +38860,7 @@
         <v>337</v>
       </c>
       <c r="B83" t="s">
-        <v>381</v>
+        <v>558</v>
       </c>
       <c r="C83">
         <v>2</v>
@@ -38856,7 +38901,7 @@
         <v>337</v>
       </c>
       <c r="B84" t="s">
-        <v>381</v>
+        <v>559</v>
       </c>
       <c r="C84">
         <v>4</v>
@@ -38897,7 +38942,7 @@
         <v>337</v>
       </c>
       <c r="B85" t="s">
-        <v>381</v>
+        <v>560</v>
       </c>
       <c r="C85">
         <v>4</v>
@@ -38938,7 +38983,7 @@
         <v>337</v>
       </c>
       <c r="B86" t="s">
-        <v>381</v>
+        <v>561</v>
       </c>
       <c r="C86">
         <v>32</v>
@@ -38979,7 +39024,7 @@
         <v>349</v>
       </c>
       <c r="B87" t="s">
-        <v>381</v>
+        <v>562</v>
       </c>
       <c r="C87">
         <v>1</v>
@@ -39020,7 +39065,7 @@
         <v>349</v>
       </c>
       <c r="B88" t="s">
-        <v>381</v>
+        <v>563</v>
       </c>
       <c r="C88">
         <v>2</v>
@@ -39061,7 +39106,7 @@
         <v>349</v>
       </c>
       <c r="B89" t="s">
-        <v>381</v>
+        <v>564</v>
       </c>
       <c r="C89">
         <v>4</v>
@@ -39102,7 +39147,7 @@
         <v>349</v>
       </c>
       <c r="B90" t="s">
-        <v>381</v>
+        <v>565</v>
       </c>
       <c r="C90">
         <v>8</v>
@@ -40741,7 +40786,7 @@
         <v>356</v>
       </c>
       <c r="B110" t="s">
-        <v>381</v>
+        <v>566</v>
       </c>
       <c r="C110">
         <v>4</v>
@@ -40782,7 +40827,7 @@
         <v>356</v>
       </c>
       <c r="B111" t="s">
-        <v>381</v>
+        <v>567</v>
       </c>
       <c r="C111">
         <v>8</v>
@@ -40823,7 +40868,7 @@
         <v>356</v>
       </c>
       <c r="B112" t="s">
-        <v>381</v>
+        <v>568</v>
       </c>
       <c r="C112">
         <v>16</v>

</xml_diff>